<commit_message>
statistics doteko 11.24, sushilki general graphics
</commit_message>
<xml_diff>
--- a/kaskad/production/sizod/zeh3linii/november/statistics11.24.xlsx
+++ b/kaskad/production/sizod/zeh3linii/november/statistics11.24.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saimkmo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Kaskad\Sambar\docs\kaskad\production\sizod\zeh3linii\november\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E04610-AC7C-4FAF-8AF7-47C260A80C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="38">
   <si>
     <t>ДОТ ЭКО</t>
   </si>
@@ -132,9 +131,6 @@
     <t>герметичность</t>
   </si>
   <si>
-    <t>Октябрь</t>
-  </si>
-  <si>
     <t>перезапуск</t>
   </si>
   <si>
@@ -148,12 +144,15 @@
   </si>
   <si>
     <t>шибер не закрылся</t>
+  </si>
+  <si>
+    <t>Ноябрь</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -820,15 +819,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -874,9 +879,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -984,9 +986,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1301,11 +1300,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,13 +1331,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="79"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1353,13 +1352,13 @@
       <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="108"/>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -1377,12 +1376,12 @@
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="107"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1401,12 +1400,12 @@
       <c r="A5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="103"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1425,12 +1424,12 @@
       <c r="A6" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="100"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="101"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1449,12 +1448,12 @@
       <c r="A7" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="96"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="97"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="98"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1473,12 +1472,12 @@
       <c r="A8" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="95"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -1497,12 +1496,12 @@
       <c r="A9" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="89" t="s">
+      <c r="B9" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="92"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1519,10 +1518,10 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="35"/>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="108"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -1557,7 +1556,7 @@
     </row>
     <row r="12" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="47" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B12" s="48">
         <v>2024</v>
@@ -1567,7 +1566,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="85" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="60" t="s">
@@ -1592,56 +1591,56 @@
       <c r="S13" s="62"/>
     </row>
     <row r="14" spans="1:19" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="85"/>
-      <c r="B14" s="80" t="s">
+      <c r="A14" s="86"/>
+      <c r="B14" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="80" t="s">
+      <c r="C14" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="64" t="s">
+      <c r="D14" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="80" t="s">
+      <c r="E14" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="69" t="s">
+      <c r="F14" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="70"/>
-      <c r="H14" s="82" t="s">
+      <c r="G14" s="72"/>
+      <c r="H14" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="83"/>
-      <c r="J14" s="87" t="s">
+      <c r="I14" s="84"/>
+      <c r="J14" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="K14" s="88"/>
-      <c r="L14" s="71" t="s">
+      <c r="K14" s="89"/>
+      <c r="L14" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="72"/>
-      <c r="N14" s="67" t="s">
+      <c r="M14" s="74"/>
+      <c r="N14" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="O14" s="68"/>
-      <c r="P14" s="73" t="s">
+      <c r="O14" s="70"/>
+      <c r="P14" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="63" t="s">
+      <c r="Q14" s="76"/>
+      <c r="R14" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="S14" s="118" t="s">
+      <c r="S14" s="63" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="86"/>
-      <c r="B15" s="81"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="81"/>
+      <c r="A15" s="87"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="64"/>
       <c r="F15" s="18" t="s">
         <v>10</v>
       </c>
@@ -1678,8 +1677,8 @@
       <c r="Q15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="R15" s="66"/>
-      <c r="S15" s="81"/>
+      <c r="R15" s="68"/>
+      <c r="S15" s="64"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="46">
@@ -1695,7 +1694,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="10">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F16" s="55" t="s">
         <v>7</v>
@@ -1710,7 +1709,7 @@
         <v>7</v>
       </c>
       <c r="J16" s="27">
-        <v>0.83</v>
+        <v>0.08</v>
       </c>
       <c r="K16" s="28" t="s">
         <v>27</v>
@@ -1735,7 +1734,7 @@
       </c>
       <c r="R16" s="36">
         <f>SUM(B16,C16,D16,E16,F16,H16,J16,L16,N16,P16)</f>
-        <v>1.75</v>
+        <v>0.74999999999999989</v>
       </c>
       <c r="S16" s="38" t="s">
         <v>29</v>
@@ -1770,7 +1769,7 @@
         <v>7</v>
       </c>
       <c r="J17" s="27">
-        <v>0.42</v>
+        <v>0.08</v>
       </c>
       <c r="K17" s="28" t="s">
         <v>27</v>
@@ -1795,7 +1794,7 @@
       </c>
       <c r="R17" s="37">
         <f t="shared" ref="R17:R32" si="0">SUM(B17,C17,D17,E17,F17,H17,J17,L17,N17,P17)</f>
-        <v>0.42</v>
+        <v>0.08</v>
       </c>
       <c r="S17" s="38" t="s">
         <v>29</v>
@@ -1865,24 +1864,24 @@
       <c r="A19" s="11">
         <v>45600</v>
       </c>
-      <c r="B19" s="109" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="110"/>
-      <c r="K19" s="110"/>
-      <c r="L19" s="110"/>
-      <c r="M19" s="110"/>
-      <c r="N19" s="110"/>
-      <c r="O19" s="110"/>
-      <c r="P19" s="110"/>
-      <c r="Q19" s="111"/>
+      <c r="B19" s="110" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="111"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="111"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="111"/>
+      <c r="K19" s="111"/>
+      <c r="L19" s="111"/>
+      <c r="M19" s="111"/>
+      <c r="N19" s="111"/>
+      <c r="O19" s="111"/>
+      <c r="P19" s="111"/>
+      <c r="Q19" s="112"/>
       <c r="R19" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1898,8 +1897,8 @@
       <c r="B20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="10">
-        <v>0.75</v>
+      <c r="C20" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>7</v>
@@ -1945,7 +1944,7 @@
       </c>
       <c r="R20" s="37">
         <f t="shared" si="0"/>
-        <v>0.92</v>
+        <v>0.17</v>
       </c>
       <c r="S20" s="38" t="s">
         <v>29</v>
@@ -2001,7 +2000,7 @@
         <v>0.09</v>
       </c>
       <c r="Q21" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R21" s="37">
         <f t="shared" si="0"/>
@@ -2019,7 +2018,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="10">
-        <v>0.34</v>
+        <v>0.17</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>7</v>
@@ -2045,8 +2044,8 @@
       <c r="K22" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="L22" s="41">
-        <v>0.17</v>
+      <c r="L22" s="41" t="s">
+        <v>7</v>
       </c>
       <c r="M22" s="41" t="s">
         <v>7</v>
@@ -2061,11 +2060,11 @@
         <v>0.17</v>
       </c>
       <c r="Q22" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R22" s="37">
         <f>SUM(B22,C22,D22,E22,F22,H22,J22,L22,N22,P22)</f>
-        <v>0.85000000000000009</v>
+        <v>0.51</v>
       </c>
       <c r="S22" s="38" t="s">
         <v>29</v>
@@ -2078,8 +2077,8 @@
       <c r="B23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="10">
-        <v>1.25</v>
+      <c r="C23" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="D23" s="9">
         <v>0.67</v>
@@ -2100,7 +2099,7 @@
         <v>7</v>
       </c>
       <c r="J23" s="27">
-        <v>0.25</v>
+        <v>0.17</v>
       </c>
       <c r="K23" s="28" t="s">
         <v>27</v>
@@ -2121,11 +2120,11 @@
         <v>0.09</v>
       </c>
       <c r="Q23" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R23" s="37">
         <f t="shared" si="0"/>
-        <v>2.59</v>
+        <v>1.26</v>
       </c>
       <c r="S23" s="38" t="s">
         <v>29</v>
@@ -2144,8 +2143,8 @@
       <c r="D24" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="10">
-        <v>0.5</v>
+      <c r="E24" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="F24" s="55" t="s">
         <v>7</v>
@@ -2165,8 +2164,8 @@
       <c r="K24" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="L24" s="41">
-        <v>0.5</v>
+      <c r="L24" s="41" t="s">
+        <v>7</v>
       </c>
       <c r="M24" s="41" t="s">
         <v>7</v>
@@ -2177,15 +2176,15 @@
       <c r="O24" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="P24" s="10">
-        <v>0.92</v>
+      <c r="P24" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="Q24" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R24" s="37">
         <f t="shared" si="0"/>
-        <v>2.34</v>
+        <v>0.42000000000000004</v>
       </c>
       <c r="S24" s="38" t="s">
         <v>29</v>
@@ -2238,14 +2237,14 @@
         <v>7</v>
       </c>
       <c r="P25" s="10">
-        <v>1.83</v>
+        <v>0.5</v>
       </c>
       <c r="Q25" s="10" t="s">
         <v>31</v>
       </c>
       <c r="R25" s="37">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0.67</v>
       </c>
       <c r="S25" s="38" t="s">
         <v>29</v>
@@ -2259,7 +2258,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="10">
-        <v>0.67</v>
+        <v>0.17</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>7</v>
@@ -2280,7 +2279,7 @@
         <v>7</v>
       </c>
       <c r="J26" s="27">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="K26" s="27" t="s">
         <v>27</v>
@@ -2301,11 +2300,11 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="Q26" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R26" s="37">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>0.83</v>
       </c>
       <c r="S26" s="38" t="s">
         <v>29</v>
@@ -2460,10 +2459,10 @@
         <v>7</v>
       </c>
       <c r="J29" s="27">
-        <v>1.67</v>
+        <v>0.5</v>
       </c>
       <c r="K29" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L29" s="41" t="s">
         <v>7</v>
@@ -2478,14 +2477,14 @@
         <v>7</v>
       </c>
       <c r="P29" s="10">
-        <v>1.67</v>
+        <v>0.25</v>
       </c>
       <c r="Q29" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R29" s="37">
         <f t="shared" si="0"/>
-        <v>3.34</v>
+        <v>0.75</v>
       </c>
       <c r="S29" s="38" t="s">
         <v>29</v>
@@ -2558,8 +2557,8 @@
       <c r="B31" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="10">
-        <v>1.34</v>
+      <c r="C31" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>7</v>
@@ -2605,7 +2604,7 @@
       </c>
       <c r="R31" s="37">
         <f>SUM(B31,C31,D31,E31,F31,H31,J31,L31,N31,P31)</f>
-        <v>1.6700000000000002</v>
+        <v>0.33</v>
       </c>
       <c r="S31" s="38" t="s">
         <v>29</v>
@@ -2657,15 +2656,15 @@
       <c r="O32" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="P32" s="10">
-        <v>0.83</v>
+      <c r="P32" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="Q32" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R32" s="37">
         <f t="shared" si="0"/>
-        <v>1.4899999999999998</v>
+        <v>0.65999999999999992</v>
       </c>
       <c r="S32" s="38" t="s">
         <v>29</v>
@@ -2678,8 +2677,8 @@
       <c r="B33" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="10">
-        <v>0.83</v>
+      <c r="C33" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>7</v>
@@ -2721,11 +2720,11 @@
         <v>0.17</v>
       </c>
       <c r="Q33" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R33" s="37">
         <f t="shared" ref="R33:R44" si="1">SUM(B33,C33,D33,E33,F33,H33,J33,L33,N33,P33)</f>
-        <v>1.17</v>
+        <v>0.34</v>
       </c>
       <c r="S33" s="38" t="s">
         <v>29</v>
@@ -2739,7 +2738,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="10">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>7</v>
@@ -2760,7 +2759,7 @@
         <v>7</v>
       </c>
       <c r="J34" s="27">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="K34" s="27" t="s">
         <v>27</v>
@@ -2781,11 +2780,11 @@
         <v>0.25</v>
       </c>
       <c r="Q34" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R34" s="37">
         <f t="shared" si="1"/>
-        <v>1.42</v>
+        <v>1.08</v>
       </c>
       <c r="S34" s="38" t="s">
         <v>29</v>
@@ -2858,14 +2857,14 @@
       <c r="B36" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="10">
-        <v>0.75</v>
+      <c r="C36" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E36" s="10">
-        <v>0.83</v>
+        <v>0.17</v>
       </c>
       <c r="F36" s="55" t="s">
         <v>7</v>
@@ -2905,7 +2904,7 @@
       </c>
       <c r="R36" s="37">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>0.34</v>
       </c>
       <c r="S36" s="38" t="s">
         <v>29</v>
@@ -2957,15 +2956,15 @@
       <c r="O37" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="P37" s="10">
-        <v>1.5</v>
+      <c r="P37" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="Q37" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R37" s="37">
         <f t="shared" si="1"/>
-        <v>1.67</v>
+        <v>0.17</v>
       </c>
       <c r="S37" s="38" t="s">
         <v>29</v>
@@ -2979,7 +2978,7 @@
         <v>7</v>
       </c>
       <c r="C38" s="10">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>7</v>
@@ -3000,7 +2999,7 @@
         <v>7</v>
       </c>
       <c r="J38" s="27">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="K38" s="27" t="s">
         <v>27</v>
@@ -3009,7 +3008,7 @@
         <v>0.17</v>
       </c>
       <c r="M38" s="41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N38" s="34" t="s">
         <v>7</v>
@@ -3025,7 +3024,7 @@
       </c>
       <c r="R38" s="37">
         <f t="shared" si="1"/>
-        <v>1.01</v>
+        <v>0.67</v>
       </c>
       <c r="S38" s="38" t="s">
         <v>29</v>
@@ -3060,7 +3059,7 @@
         <v>7</v>
       </c>
       <c r="J39" s="27">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="K39" s="27" t="s">
         <v>27</v>
@@ -3085,7 +3084,7 @@
       </c>
       <c r="R39" s="37">
         <f t="shared" si="1"/>
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="S39" s="38" t="s">
         <v>29</v>
@@ -3120,7 +3119,7 @@
         <v>7</v>
       </c>
       <c r="J40" s="27">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="K40" s="27" t="s">
         <v>27</v>
@@ -3137,15 +3136,15 @@
       <c r="O40" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="P40" s="10">
-        <v>0.8</v>
+      <c r="P40" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="Q40" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R40" s="37">
         <f t="shared" si="1"/>
-        <v>1.05</v>
+        <v>0.08</v>
       </c>
       <c r="S40" s="38" t="s">
         <v>29</v>
@@ -3159,13 +3158,13 @@
         <v>7</v>
       </c>
       <c r="C41" s="10">
-        <v>0.41</v>
+        <v>0.17</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E41" s="10">
-        <v>1</v>
+        <v>0.17</v>
       </c>
       <c r="F41" s="45" t="s">
         <v>7</v>
@@ -3180,7 +3179,7 @@
         <v>7</v>
       </c>
       <c r="J41" s="27">
-        <v>0.25</v>
+        <v>0.08</v>
       </c>
       <c r="K41" s="27" t="s">
         <v>27</v>
@@ -3205,7 +3204,7 @@
       </c>
       <c r="R41" s="37">
         <f t="shared" si="1"/>
-        <v>1.8299999999999998</v>
+        <v>0.59000000000000008</v>
       </c>
       <c r="S41" s="38" t="s">
         <v>29</v>
@@ -3240,7 +3239,7 @@
         <v>7</v>
       </c>
       <c r="J42" s="27">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="K42" s="27" t="s">
         <v>27</v>
@@ -3258,14 +3257,14 @@
         <v>7</v>
       </c>
       <c r="P42" s="10">
-        <v>0.34</v>
+        <v>0.42</v>
       </c>
       <c r="Q42" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R42" s="37">
         <f t="shared" si="1"/>
-        <v>0.76</v>
+        <v>0.75</v>
       </c>
       <c r="S42" s="38" t="s">
         <v>29</v>
@@ -3279,13 +3278,13 @@
         <v>7</v>
       </c>
       <c r="C43" s="10">
-        <v>0.57999999999999996</v>
+        <v>0.25</v>
       </c>
       <c r="D43" s="9">
-        <v>1.83</v>
+        <v>0.83</v>
       </c>
       <c r="E43" s="10">
-        <v>0.57999999999999996</v>
+        <v>0.25</v>
       </c>
       <c r="F43" s="45" t="s">
         <v>7</v>
@@ -3321,11 +3320,11 @@
         <v>0.08</v>
       </c>
       <c r="Q43" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R43" s="37">
         <f t="shared" si="1"/>
-        <v>3.24</v>
+        <v>1.58</v>
       </c>
       <c r="S43" s="38" t="s">
         <v>29</v>
@@ -3360,7 +3359,7 @@
         <v>7</v>
       </c>
       <c r="J44" s="27">
-        <v>0.17</v>
+        <v>0.08</v>
       </c>
       <c r="K44" s="27" t="s">
         <v>27</v>
@@ -3385,7 +3384,7 @@
       </c>
       <c r="R44" s="37">
         <f t="shared" si="1"/>
-        <v>0.42000000000000004</v>
+        <v>0.33</v>
       </c>
       <c r="S44" s="38" t="s">
         <v>29</v>
@@ -3438,14 +3437,14 @@
         <v>7</v>
       </c>
       <c r="P45" s="12">
-        <v>0.33</v>
+        <v>0.15</v>
       </c>
       <c r="Q45" s="43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R45" s="37">
         <f t="shared" ref="R45" si="2">SUM(B45,C45,D45,E45,F45,H45,J45,L45,N45,P45)</f>
-        <v>1</v>
+        <v>0.82000000000000006</v>
       </c>
       <c r="S45" s="38" t="s">
         <v>29</v>
@@ -3461,51 +3460,51 @@
       </c>
       <c r="C46" s="52">
         <f>SUM(C16:C45)</f>
-        <v>10</v>
+        <v>3.34</v>
       </c>
       <c r="D46" s="54">
         <f>SUM(D16:D45)</f>
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="E46" s="54">
         <f>SUM(E16:E45)</f>
-        <v>5.41</v>
-      </c>
-      <c r="F46" s="116">
+        <v>2.84</v>
+      </c>
+      <c r="F46" s="117">
         <f>SUM(F16:F45)</f>
         <v>0</v>
       </c>
-      <c r="G46" s="117"/>
-      <c r="H46" s="116">
+      <c r="G46" s="118"/>
+      <c r="H46" s="117">
         <f>SUM(H16:H45)</f>
         <v>0</v>
       </c>
-      <c r="I46" s="117"/>
-      <c r="J46" s="112">
+      <c r="I46" s="118"/>
+      <c r="J46" s="113">
         <f>SUM(J16:J45)</f>
-        <v>7.6499999999999986</v>
-      </c>
-      <c r="K46" s="113"/>
-      <c r="L46" s="112">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="K46" s="114"/>
+      <c r="L46" s="113">
         <f>SUM(L16:L45)</f>
-        <v>1.26</v>
-      </c>
-      <c r="M46" s="113"/>
-      <c r="N46" s="112">
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="M46" s="114"/>
+      <c r="N46" s="113">
         <f>SUM(N16:N45)</f>
         <v>0</v>
       </c>
-      <c r="O46" s="113"/>
-      <c r="P46" s="78">
+      <c r="O46" s="114"/>
+      <c r="P46" s="80">
         <f>SUM(P16:P45)</f>
-        <v>10.7</v>
-      </c>
-      <c r="Q46" s="79"/>
-      <c r="R46" s="114">
+        <v>3.8000000000000003</v>
+      </c>
+      <c r="Q46" s="81"/>
+      <c r="R46" s="115">
         <f>SUM(R16:R45)</f>
-        <v>37.520000000000003</v>
-      </c>
-      <c r="S46" s="115"/>
+        <v>16.420000000000002</v>
+      </c>
+      <c r="S46" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="31">

</xml_diff>